<commit_message>
test result of  automation
test result of  automation
</commit_message>
<xml_diff>
--- a/PCB/04 Dev_Lib/4.4_Unit Test/Test Result (LULU)__Sprint2_20151004 .xlsx
+++ b/PCB/04 Dev_Lib/4.4_Unit Test/Test Result (LULU)__Sprint2_20151004 .xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Relevant Tests</t>
   </si>
@@ -40,85 +40,78 @@
     <t>1.4.</t>
   </si>
   <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>2.2.</t>
+  </si>
+  <si>
+    <t>2.3.</t>
+  </si>
+  <si>
+    <t>2.4.</t>
+  </si>
+  <si>
+    <t>2.1.</t>
+  </si>
+  <si>
+    <t>The header of list page should be the common component.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The footer of list page should be the common component.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The link "Test Automation" can work correctly.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All of information should be displayed in TestAutomation page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The picture should be displayed </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The link "About Getskills” can response correctly. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automation page for browser view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Automation Page (mobile phone and browser view).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automation page for mobile phone view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Put URL (TestAutomation page) in the test website </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">All pictures and contexts should adapt the users form phone </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All pictures and context should be displayed on mobile phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Touching"TestAuomation"on homepage, Automationpage can displayed </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.5.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1.6.</t>
-  </si>
-  <si>
-    <t>1.7.</t>
-  </si>
-  <si>
-    <t>The default list of success stories includes all the active data.</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>2.2.</t>
-  </si>
-  <si>
-    <t>2.3.</t>
-  </si>
-  <si>
-    <t>2.4.</t>
-  </si>
-  <si>
-    <t>2.1.</t>
-  </si>
-  <si>
-    <t>User story 2: Dynamic team profile page (client view).</t>
-  </si>
-  <si>
-    <t>The header of list page should be the common component.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The footer of list page should be the common component.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The link "Test Automation" can work correctly.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All of information should be displayed in TestAutomation page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The picture should be displayed </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The link "About Getskills” can response correctly. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Automation page for browser view</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test Automation Page (mobile phone and browser view).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Automation page for mobile phone view</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Put URL (TestAutomation page) in the test website </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">All pictures and contexts should adapt the users form phone </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All pictures and context should be displayed on mobile phone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Touching"TestAuomation"on homepage, Automationpage can displayed </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AK21"/>
+  <dimension ref="B2:AK20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -588,7 +581,7 @@
   <sheetData>
     <row r="2" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -638,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -682,7 +675,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -726,7 +719,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -770,7 +763,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -814,7 +807,7 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -854,11 +847,11 @@
     <row r="9" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="C9" s="9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -898,11 +891,11 @@
     <row r="10" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B10" s="2"/>
       <c r="C10" s="9" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -940,143 +933,136 @@
       <c r="AK10" s="4"/>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="B11" s="2"/>
-      <c r="C11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="4"/>
-      <c r="AB11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="3"/>
-      <c r="AK11" s="4"/>
-    </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="7"/>
-    </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="10" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="7"/>
+    </row>
+    <row r="14" spans="2:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="11" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="12"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="12"/>
+    </row>
+    <row r="15" spans="2:37" x14ac:dyDescent="0.15">
+      <c r="B15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="4"/>
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1099,7 +1085,9 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="4"/>
-      <c r="AB16" s="3"/>
+      <c r="AB16" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
@@ -1113,11 +1101,11 @@
     <row r="17" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B17" s="2"/>
       <c r="C17" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1157,11 +1145,11 @@
     <row r="18" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B18" s="2"/>
       <c r="C18" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1201,11 +1189,11 @@
     <row r="19" spans="2:37" x14ac:dyDescent="0.15">
       <c r="B19" s="2"/>
       <c r="C19" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1243,86 +1231,42 @@
       <c r="AK19" s="4"/>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="B20" s="2"/>
-      <c r="C20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
-      <c r="AK20" s="4"/>
-    </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.15">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="6"/>
-      <c r="AG21" s="6"/>
-      <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="7"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>